<commit_message>
Corrections through Lamborghini. Correction File Migrating Algorithm done, needs testing.
</commit_message>
<xml_diff>
--- a/Docs/CorrectionStatus.xlsx
+++ b/Docs/CorrectionStatus.xlsx
@@ -1125,15 +1125,15 @@
       <c r="U5" s="5" t="n"/>
       <c r="V5" s="5" t="n"/>
       <c r="W5" s="5" t="n"/>
-      <c r="X5" s="3" t="n"/>
-      <c r="Y5" s="3" t="n"/>
-      <c r="Z5" s="3" t="n"/>
-      <c r="AA5" s="3" t="n"/>
-      <c r="AB5" s="3" t="n"/>
-      <c r="AC5" s="3" t="n"/>
-      <c r="AD5" s="3" t="n"/>
+      <c r="X5" s="5" t="n"/>
+      <c r="Y5" s="5" t="n"/>
+      <c r="Z5" s="5" t="n"/>
+      <c r="AA5" s="5" t="n"/>
+      <c r="AB5" s="5" t="n"/>
+      <c r="AC5" s="5" t="n"/>
+      <c r="AD5" s="5" t="n"/>
       <c r="AE5" s="4" t="n"/>
-      <c r="AF5" s="3" t="n"/>
+      <c r="AF5" s="5" t="n"/>
       <c r="AG5" s="3" t="n"/>
       <c r="AH5" s="3" t="n"/>
       <c r="AI5" s="3" t="n"/>
@@ -1201,15 +1201,15 @@
       <c r="U6" s="5" t="n"/>
       <c r="V6" s="5" t="n"/>
       <c r="W6" s="5" t="n"/>
-      <c r="X6" s="3" t="n"/>
-      <c r="Y6" s="3" t="n"/>
-      <c r="Z6" s="3" t="n"/>
-      <c r="AA6" s="3" t="n"/>
-      <c r="AB6" s="3" t="n"/>
-      <c r="AC6" s="3" t="n"/>
-      <c r="AD6" s="3" t="n"/>
+      <c r="X6" s="5" t="n"/>
+      <c r="Y6" s="5" t="n"/>
+      <c r="Z6" s="5" t="n"/>
+      <c r="AA6" s="5" t="n"/>
+      <c r="AB6" s="5" t="n"/>
+      <c r="AC6" s="5" t="n"/>
+      <c r="AD6" s="5" t="n"/>
       <c r="AE6" s="4" t="n"/>
-      <c r="AF6" s="3" t="n"/>
+      <c r="AF6" s="5" t="n"/>
       <c r="AG6" s="3" t="n"/>
       <c r="AH6" s="3" t="n"/>
       <c r="AI6" s="3" t="n"/>
@@ -1277,15 +1277,15 @@
       <c r="U7" s="5" t="n"/>
       <c r="V7" s="5" t="n"/>
       <c r="W7" s="5" t="n"/>
-      <c r="X7" s="3" t="n"/>
-      <c r="Y7" s="3" t="n"/>
-      <c r="Z7" s="3" t="n"/>
-      <c r="AA7" s="3" t="n"/>
-      <c r="AB7" s="3" t="n"/>
-      <c r="AC7" s="3" t="n"/>
-      <c r="AD7" s="3" t="n"/>
+      <c r="X7" s="5" t="n"/>
+      <c r="Y7" s="5" t="n"/>
+      <c r="Z7" s="5" t="n"/>
+      <c r="AA7" s="5" t="n"/>
+      <c r="AB7" s="5" t="n"/>
+      <c r="AC7" s="5" t="n"/>
+      <c r="AD7" s="5" t="n"/>
       <c r="AE7" s="4" t="n"/>
-      <c r="AF7" s="3" t="n"/>
+      <c r="AF7" s="5" t="n"/>
       <c r="AG7" s="3" t="n"/>
       <c r="AH7" s="3" t="n"/>
       <c r="AI7" s="3" t="n"/>
@@ -1962,14 +1962,14 @@
       <c r="V16" s="3" t="n"/>
       <c r="W16" s="5" t="n"/>
       <c r="X16" s="3" t="n"/>
-      <c r="Y16" s="3" t="n"/>
-      <c r="Z16" s="3" t="n"/>
-      <c r="AA16" s="3" t="n"/>
-      <c r="AB16" s="3" t="n"/>
+      <c r="Y16" s="5" t="n"/>
+      <c r="Z16" s="5" t="n"/>
+      <c r="AA16" s="5" t="n"/>
+      <c r="AB16" s="5" t="n"/>
       <c r="AC16" s="3" t="n"/>
-      <c r="AD16" s="3" t="n"/>
+      <c r="AD16" s="5" t="n"/>
       <c r="AE16" s="4" t="n"/>
-      <c r="AF16" s="3" t="n"/>
+      <c r="AF16" s="5" t="n"/>
       <c r="AG16" s="3" t="n"/>
       <c r="AH16" s="3" t="n"/>
       <c r="AI16" s="3" t="n"/>
@@ -2721,15 +2721,15 @@
       <c r="U26" s="5" t="n"/>
       <c r="V26" s="5" t="n"/>
       <c r="W26" s="5" t="n"/>
-      <c r="X26" s="3" t="n"/>
-      <c r="Y26" s="3" t="n"/>
-      <c r="Z26" s="3" t="n"/>
-      <c r="AA26" s="3" t="n"/>
-      <c r="AB26" s="3" t="n"/>
-      <c r="AC26" s="3" t="n"/>
-      <c r="AD26" s="3" t="n"/>
+      <c r="X26" s="5" t="n"/>
+      <c r="Y26" s="5" t="n"/>
+      <c r="Z26" s="5" t="n"/>
+      <c r="AA26" s="5" t="n"/>
+      <c r="AB26" s="5" t="n"/>
+      <c r="AC26" s="5" t="n"/>
+      <c r="AD26" s="5" t="n"/>
       <c r="AE26" s="4" t="n"/>
-      <c r="AF26" s="3" t="n"/>
+      <c r="AF26" s="5" t="n"/>
       <c r="AG26" s="3" t="n"/>
       <c r="AH26" s="3" t="n"/>
       <c r="AI26" s="3" t="n"/>

</xml_diff>

<commit_message>
More Corrections, added definition for better lint typecasting
</commit_message>
<xml_diff>
--- a/Docs/CorrectionStatus.xlsx
+++ b/Docs/CorrectionStatus.xlsx
@@ -1134,25 +1134,25 @@
       <c r="AD5" s="5" t="n"/>
       <c r="AE5" s="4" t="n"/>
       <c r="AF5" s="5" t="n"/>
-      <c r="AG5" s="3" t="n"/>
-      <c r="AH5" s="3" t="n"/>
-      <c r="AI5" s="3" t="n"/>
-      <c r="AJ5" s="3" t="n"/>
-      <c r="AK5" s="3" t="n"/>
+      <c r="AG5" s="5" t="n"/>
+      <c r="AH5" s="5" t="n"/>
+      <c r="AI5" s="5" t="n"/>
+      <c r="AJ5" s="5" t="n"/>
+      <c r="AK5" s="5" t="n"/>
       <c r="AL5" s="4" t="n"/>
-      <c r="AM5" s="3" t="n"/>
-      <c r="AN5" s="3" t="n"/>
-      <c r="AO5" s="3" t="n"/>
-      <c r="AP5" s="3" t="n"/>
-      <c r="AQ5" s="3" t="n"/>
-      <c r="AR5" s="3" t="n"/>
-      <c r="AS5" s="3" t="n"/>
-      <c r="AT5" s="3" t="n"/>
-      <c r="AU5" s="3" t="n"/>
+      <c r="AM5" s="5" t="n"/>
+      <c r="AN5" s="5" t="n"/>
+      <c r="AO5" s="5" t="n"/>
+      <c r="AP5" s="5" t="n"/>
+      <c r="AQ5" s="5" t="n"/>
+      <c r="AR5" s="5" t="n"/>
+      <c r="AS5" s="5" t="n"/>
+      <c r="AT5" s="5" t="n"/>
+      <c r="AU5" s="5" t="n"/>
       <c r="AV5" s="4" t="n"/>
       <c r="AW5" s="3" t="n"/>
       <c r="AX5" s="4" t="n"/>
-      <c r="AY5" s="3" t="n"/>
+      <c r="AY5" s="5" t="n"/>
       <c r="AZ5" s="3" t="n"/>
       <c r="BA5" s="3" t="n"/>
       <c r="BB5" s="3" t="n"/>
@@ -1210,25 +1210,25 @@
       <c r="AD6" s="5" t="n"/>
       <c r="AE6" s="4" t="n"/>
       <c r="AF6" s="5" t="n"/>
-      <c r="AG6" s="3" t="n"/>
-      <c r="AH6" s="3" t="n"/>
-      <c r="AI6" s="3" t="n"/>
-      <c r="AJ6" s="3" t="n"/>
-      <c r="AK6" s="3" t="n"/>
+      <c r="AG6" s="5" t="n"/>
+      <c r="AH6" s="5" t="n"/>
+      <c r="AI6" s="5" t="n"/>
+      <c r="AJ6" s="5" t="n"/>
+      <c r="AK6" s="5" t="n"/>
       <c r="AL6" s="4" t="n"/>
-      <c r="AM6" s="3" t="n"/>
-      <c r="AN6" s="3" t="n"/>
-      <c r="AO6" s="3" t="n"/>
-      <c r="AP6" s="3" t="n"/>
-      <c r="AQ6" s="3" t="n"/>
-      <c r="AR6" s="3" t="n"/>
-      <c r="AS6" s="3" t="n"/>
-      <c r="AT6" s="3" t="n"/>
-      <c r="AU6" s="3" t="n"/>
+      <c r="AM6" s="5" t="n"/>
+      <c r="AN6" s="5" t="n"/>
+      <c r="AO6" s="5" t="n"/>
+      <c r="AP6" s="5" t="n"/>
+      <c r="AQ6" s="5" t="n"/>
+      <c r="AR6" s="5" t="n"/>
+      <c r="AS6" s="5" t="n"/>
+      <c r="AT6" s="5" t="n"/>
+      <c r="AU6" s="5" t="n"/>
       <c r="AV6" s="4" t="n"/>
       <c r="AW6" s="3" t="n"/>
       <c r="AX6" s="4" t="n"/>
-      <c r="AY6" s="3" t="n"/>
+      <c r="AY6" s="5" t="n"/>
       <c r="AZ6" s="3" t="n"/>
       <c r="BA6" s="3" t="n"/>
       <c r="BB6" s="3" t="n"/>
@@ -1286,25 +1286,25 @@
       <c r="AD7" s="5" t="n"/>
       <c r="AE7" s="4" t="n"/>
       <c r="AF7" s="5" t="n"/>
-      <c r="AG7" s="3" t="n"/>
-      <c r="AH7" s="3" t="n"/>
-      <c r="AI7" s="3" t="n"/>
-      <c r="AJ7" s="3" t="n"/>
-      <c r="AK7" s="3" t="n"/>
+      <c r="AG7" s="5" t="n"/>
+      <c r="AH7" s="5" t="n"/>
+      <c r="AI7" s="5" t="n"/>
+      <c r="AJ7" s="5" t="n"/>
+      <c r="AK7" s="5" t="n"/>
       <c r="AL7" s="4" t="n"/>
-      <c r="AM7" s="3" t="n"/>
-      <c r="AN7" s="3" t="n"/>
-      <c r="AO7" s="3" t="n"/>
-      <c r="AP7" s="3" t="n"/>
-      <c r="AQ7" s="3" t="n"/>
-      <c r="AR7" s="3" t="n"/>
-      <c r="AS7" s="3" t="n"/>
-      <c r="AT7" s="3" t="n"/>
-      <c r="AU7" s="3" t="n"/>
+      <c r="AM7" s="5" t="n"/>
+      <c r="AN7" s="5" t="n"/>
+      <c r="AO7" s="5" t="n"/>
+      <c r="AP7" s="5" t="n"/>
+      <c r="AQ7" s="5" t="n"/>
+      <c r="AR7" s="5" t="n"/>
+      <c r="AS7" s="5" t="n"/>
+      <c r="AT7" s="5" t="n"/>
+      <c r="AU7" s="5" t="n"/>
       <c r="AV7" s="4" t="n"/>
       <c r="AW7" s="3" t="n"/>
       <c r="AX7" s="4" t="n"/>
-      <c r="AY7" s="3" t="n"/>
+      <c r="AY7" s="5" t="n"/>
       <c r="AZ7" s="3" t="n"/>
       <c r="BA7" s="3" t="n"/>
       <c r="BB7" s="3" t="n"/>
@@ -1970,21 +1970,21 @@
       <c r="AD16" s="5" t="n"/>
       <c r="AE16" s="4" t="n"/>
       <c r="AF16" s="5" t="n"/>
-      <c r="AG16" s="3" t="n"/>
-      <c r="AH16" s="3" t="n"/>
-      <c r="AI16" s="3" t="n"/>
+      <c r="AG16" s="5" t="n"/>
+      <c r="AH16" s="5" t="n"/>
+      <c r="AI16" s="5" t="n"/>
       <c r="AJ16" s="3" t="n"/>
       <c r="AK16" s="3" t="n"/>
       <c r="AL16" s="4" t="n"/>
-      <c r="AM16" s="3" t="n"/>
-      <c r="AN16" s="3" t="n"/>
+      <c r="AM16" s="5" t="n"/>
+      <c r="AN16" s="5" t="n"/>
       <c r="AO16" s="3" t="n"/>
       <c r="AP16" s="3" t="n"/>
-      <c r="AQ16" s="3" t="n"/>
+      <c r="AQ16" s="5" t="n"/>
       <c r="AR16" s="3" t="n"/>
       <c r="AS16" s="3" t="n"/>
       <c r="AT16" s="3" t="n"/>
-      <c r="AU16" s="3" t="n"/>
+      <c r="AU16" s="5" t="n"/>
       <c r="AV16" s="4" t="n"/>
       <c r="AW16" s="3" t="n"/>
       <c r="AX16" s="4" t="n"/>
@@ -2730,25 +2730,25 @@
       <c r="AD26" s="5" t="n"/>
       <c r="AE26" s="4" t="n"/>
       <c r="AF26" s="5" t="n"/>
-      <c r="AG26" s="3" t="n"/>
-      <c r="AH26" s="3" t="n"/>
-      <c r="AI26" s="3" t="n"/>
-      <c r="AJ26" s="3" t="n"/>
-      <c r="AK26" s="3" t="n"/>
+      <c r="AG26" s="5" t="n"/>
+      <c r="AH26" s="5" t="n"/>
+      <c r="AI26" s="5" t="n"/>
+      <c r="AJ26" s="5" t="n"/>
+      <c r="AK26" s="5" t="n"/>
       <c r="AL26" s="4" t="n"/>
-      <c r="AM26" s="3" t="n"/>
-      <c r="AN26" s="3" t="n"/>
-      <c r="AO26" s="3" t="n"/>
-      <c r="AP26" s="3" t="n"/>
-      <c r="AQ26" s="3" t="n"/>
-      <c r="AR26" s="3" t="n"/>
-      <c r="AS26" s="3" t="n"/>
-      <c r="AT26" s="3" t="n"/>
-      <c r="AU26" s="3" t="n"/>
+      <c r="AM26" s="5" t="n"/>
+      <c r="AN26" s="5" t="n"/>
+      <c r="AO26" s="5" t="n"/>
+      <c r="AP26" s="5" t="n"/>
+      <c r="AQ26" s="5" t="n"/>
+      <c r="AR26" s="5" t="n"/>
+      <c r="AS26" s="5" t="n"/>
+      <c r="AT26" s="5" t="n"/>
+      <c r="AU26" s="5" t="n"/>
       <c r="AV26" s="4" t="n"/>
       <c r="AW26" s="3" t="n"/>
       <c r="AX26" s="4" t="n"/>
-      <c r="AY26" s="3" t="n"/>
+      <c r="AY26" s="5" t="n"/>
       <c r="AZ26" s="3" t="n"/>
       <c r="BA26" s="3" t="n"/>
       <c r="BB26" s="3" t="n"/>

</xml_diff>

<commit_message>
Corrections up to and including Smart. Subaru-Volvo left
</commit_message>
<xml_diff>
--- a/Docs/CorrectionStatus.xlsx
+++ b/Docs/CorrectionStatus.xlsx
@@ -1150,20 +1150,20 @@
       <c r="AT5" s="5" t="n"/>
       <c r="AU5" s="5" t="n"/>
       <c r="AV5" s="4" t="n"/>
-      <c r="AW5" s="3" t="n"/>
+      <c r="AW5" s="5" t="n"/>
       <c r="AX5" s="4" t="n"/>
       <c r="AY5" s="5" t="n"/>
-      <c r="AZ5" s="3" t="n"/>
-      <c r="BA5" s="3" t="n"/>
-      <c r="BB5" s="3" t="n"/>
+      <c r="AZ5" s="5" t="n"/>
+      <c r="BA5" s="5" t="n"/>
+      <c r="BB5" s="5" t="n"/>
       <c r="BC5" s="4" t="n"/>
-      <c r="BD5" s="3" t="n"/>
-      <c r="BE5" s="3" t="n"/>
-      <c r="BF5" s="3" t="n"/>
-      <c r="BG5" s="3" t="n"/>
-      <c r="BH5" s="3" t="n"/>
+      <c r="BD5" s="5" t="n"/>
+      <c r="BE5" s="5" t="n"/>
+      <c r="BF5" s="5" t="n"/>
+      <c r="BG5" s="5" t="n"/>
+      <c r="BH5" s="5" t="n"/>
       <c r="BI5" s="4" t="n"/>
-      <c r="BJ5" s="3" t="n"/>
+      <c r="BJ5" s="5" t="n"/>
       <c r="BK5" s="4" t="n"/>
       <c r="BL5" s="3" t="n"/>
       <c r="BM5" s="3" t="n"/>
@@ -1226,20 +1226,20 @@
       <c r="AT6" s="5" t="n"/>
       <c r="AU6" s="5" t="n"/>
       <c r="AV6" s="4" t="n"/>
-      <c r="AW6" s="3" t="n"/>
+      <c r="AW6" s="5" t="n"/>
       <c r="AX6" s="4" t="n"/>
       <c r="AY6" s="5" t="n"/>
-      <c r="AZ6" s="3" t="n"/>
-      <c r="BA6" s="3" t="n"/>
-      <c r="BB6" s="3" t="n"/>
+      <c r="AZ6" s="5" t="n"/>
+      <c r="BA6" s="5" t="n"/>
+      <c r="BB6" s="5" t="n"/>
       <c r="BC6" s="4" t="n"/>
-      <c r="BD6" s="3" t="n"/>
-      <c r="BE6" s="3" t="n"/>
-      <c r="BF6" s="3" t="n"/>
-      <c r="BG6" s="3" t="n"/>
-      <c r="BH6" s="3" t="n"/>
+      <c r="BD6" s="5" t="n"/>
+      <c r="BE6" s="5" t="n"/>
+      <c r="BF6" s="5" t="n"/>
+      <c r="BG6" s="5" t="n"/>
+      <c r="BH6" s="5" t="n"/>
       <c r="BI6" s="4" t="n"/>
-      <c r="BJ6" s="3" t="n"/>
+      <c r="BJ6" s="5" t="n"/>
       <c r="BK6" s="4" t="n"/>
       <c r="BL6" s="3" t="n"/>
       <c r="BM6" s="3" t="n"/>
@@ -1302,20 +1302,20 @@
       <c r="AT7" s="5" t="n"/>
       <c r="AU7" s="5" t="n"/>
       <c r="AV7" s="4" t="n"/>
-      <c r="AW7" s="3" t="n"/>
+      <c r="AW7" s="5" t="n"/>
       <c r="AX7" s="4" t="n"/>
       <c r="AY7" s="5" t="n"/>
-      <c r="AZ7" s="3" t="n"/>
-      <c r="BA7" s="3" t="n"/>
-      <c r="BB7" s="3" t="n"/>
+      <c r="AZ7" s="5" t="n"/>
+      <c r="BA7" s="5" t="n"/>
+      <c r="BB7" s="5" t="n"/>
       <c r="BC7" s="4" t="n"/>
-      <c r="BD7" s="3" t="n"/>
-      <c r="BE7" s="3" t="n"/>
-      <c r="BF7" s="3" t="n"/>
-      <c r="BG7" s="3" t="n"/>
-      <c r="BH7" s="3" t="n"/>
+      <c r="BD7" s="5" t="n"/>
+      <c r="BE7" s="5" t="n"/>
+      <c r="BF7" s="5" t="n"/>
+      <c r="BG7" s="5" t="n"/>
+      <c r="BH7" s="5" t="n"/>
       <c r="BI7" s="4" t="n"/>
-      <c r="BJ7" s="3" t="n"/>
+      <c r="BJ7" s="5" t="n"/>
       <c r="BK7" s="4" t="n"/>
       <c r="BL7" s="3" t="n"/>
       <c r="BM7" s="3" t="n"/>
@@ -1990,16 +1990,16 @@
       <c r="AX16" s="4" t="n"/>
       <c r="AY16" s="3" t="n"/>
       <c r="AZ16" s="3" t="n"/>
-      <c r="BA16" s="3" t="n"/>
+      <c r="BA16" s="5" t="n"/>
       <c r="BB16" s="3" t="n"/>
       <c r="BC16" s="4" t="n"/>
       <c r="BD16" s="3" t="n"/>
       <c r="BE16" s="3" t="n"/>
-      <c r="BF16" s="3" t="n"/>
+      <c r="BF16" s="5" t="n"/>
       <c r="BG16" s="3" t="n"/>
-      <c r="BH16" s="3" t="n"/>
+      <c r="BH16" s="5" t="n"/>
       <c r="BI16" s="4" t="n"/>
-      <c r="BJ16" s="3" t="n"/>
+      <c r="BJ16" s="5" t="n"/>
       <c r="BK16" s="4" t="n"/>
       <c r="BL16" s="3" t="n"/>
       <c r="BM16" s="3" t="n"/>
@@ -2746,20 +2746,20 @@
       <c r="AT26" s="5" t="n"/>
       <c r="AU26" s="5" t="n"/>
       <c r="AV26" s="4" t="n"/>
-      <c r="AW26" s="3" t="n"/>
+      <c r="AW26" s="5" t="n"/>
       <c r="AX26" s="4" t="n"/>
       <c r="AY26" s="5" t="n"/>
-      <c r="AZ26" s="3" t="n"/>
-      <c r="BA26" s="3" t="n"/>
-      <c r="BB26" s="3" t="n"/>
+      <c r="AZ26" s="5" t="n"/>
+      <c r="BA26" s="5" t="n"/>
+      <c r="BB26" s="5" t="n"/>
       <c r="BC26" s="4" t="n"/>
-      <c r="BD26" s="3" t="n"/>
-      <c r="BE26" s="3" t="n"/>
-      <c r="BF26" s="3" t="n"/>
-      <c r="BG26" s="3" t="n"/>
-      <c r="BH26" s="3" t="n"/>
+      <c r="BD26" s="5" t="n"/>
+      <c r="BE26" s="5" t="n"/>
+      <c r="BF26" s="5" t="n"/>
+      <c r="BG26" s="5" t="n"/>
+      <c r="BH26" s="5" t="n"/>
       <c r="BI26" s="4" t="n"/>
-      <c r="BJ26" s="3" t="n"/>
+      <c r="BJ26" s="5" t="n"/>
       <c r="BK26" s="4" t="n"/>
       <c r="BL26" s="3" t="n"/>
       <c r="BM26" s="3" t="n"/>

</xml_diff>

<commit_message>
Done with preliminary implementation of corrections
</commit_message>
<xml_diff>
--- a/Docs/CorrectionStatus.xlsx
+++ b/Docs/CorrectionStatus.xlsx
@@ -1165,13 +1165,13 @@
       <c r="BI5" s="4" t="n"/>
       <c r="BJ5" s="5" t="n"/>
       <c r="BK5" s="4" t="n"/>
-      <c r="BL5" s="3" t="n"/>
-      <c r="BM5" s="3" t="n"/>
-      <c r="BN5" s="3" t="n"/>
-      <c r="BO5" s="3" t="n"/>
-      <c r="BP5" s="3" t="n"/>
-      <c r="BQ5" s="3" t="n"/>
-      <c r="BR5" s="3" t="n"/>
+      <c r="BL5" s="5" t="n"/>
+      <c r="BM5" s="5" t="n"/>
+      <c r="BN5" s="5" t="n"/>
+      <c r="BO5" s="5" t="n"/>
+      <c r="BP5" s="5" t="n"/>
+      <c r="BQ5" s="5" t="n"/>
+      <c r="BR5" s="5" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -1241,13 +1241,13 @@
       <c r="BI6" s="4" t="n"/>
       <c r="BJ6" s="5" t="n"/>
       <c r="BK6" s="4" t="n"/>
-      <c r="BL6" s="3" t="n"/>
-      <c r="BM6" s="3" t="n"/>
-      <c r="BN6" s="3" t="n"/>
-      <c r="BO6" s="3" t="n"/>
-      <c r="BP6" s="3" t="n"/>
-      <c r="BQ6" s="3" t="n"/>
-      <c r="BR6" s="3" t="n"/>
+      <c r="BL6" s="5" t="n"/>
+      <c r="BM6" s="5" t="n"/>
+      <c r="BN6" s="5" t="n"/>
+      <c r="BO6" s="5" t="n"/>
+      <c r="BP6" s="5" t="n"/>
+      <c r="BQ6" s="5" t="n"/>
+      <c r="BR6" s="5" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
@@ -1317,13 +1317,13 @@
       <c r="BI7" s="4" t="n"/>
       <c r="BJ7" s="5" t="n"/>
       <c r="BK7" s="4" t="n"/>
-      <c r="BL7" s="3" t="n"/>
-      <c r="BM7" s="3" t="n"/>
-      <c r="BN7" s="3" t="n"/>
-      <c r="BO7" s="3" t="n"/>
-      <c r="BP7" s="3" t="n"/>
-      <c r="BQ7" s="3" t="n"/>
-      <c r="BR7" s="3" t="n"/>
+      <c r="BL7" s="5" t="n"/>
+      <c r="BM7" s="5" t="n"/>
+      <c r="BN7" s="5" t="n"/>
+      <c r="BO7" s="5" t="n"/>
+      <c r="BP7" s="5" t="n"/>
+      <c r="BQ7" s="5" t="n"/>
+      <c r="BR7" s="5" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -2001,13 +2001,13 @@
       <c r="BI16" s="4" t="n"/>
       <c r="BJ16" s="5" t="n"/>
       <c r="BK16" s="4" t="n"/>
-      <c r="BL16" s="3" t="n"/>
-      <c r="BM16" s="3" t="n"/>
+      <c r="BL16" s="5" t="n"/>
+      <c r="BM16" s="5" t="n"/>
       <c r="BN16" s="3" t="n"/>
-      <c r="BO16" s="3" t="n"/>
+      <c r="BO16" s="5" t="n"/>
       <c r="BP16" s="3" t="n"/>
-      <c r="BQ16" s="3" t="n"/>
-      <c r="BR16" s="3" t="n"/>
+      <c r="BQ16" s="5" t="n"/>
+      <c r="BR16" s="5" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
@@ -2761,13 +2761,13 @@
       <c r="BI26" s="4" t="n"/>
       <c r="BJ26" s="5" t="n"/>
       <c r="BK26" s="4" t="n"/>
-      <c r="BL26" s="3" t="n"/>
-      <c r="BM26" s="3" t="n"/>
+      <c r="BL26" s="5" t="n"/>
+      <c r="BM26" s="5" t="n"/>
       <c r="BN26" s="3" t="n"/>
-      <c r="BO26" s="3" t="n"/>
-      <c r="BP26" s="3" t="n"/>
-      <c r="BQ26" s="3" t="n"/>
-      <c r="BR26" s="3" t="n"/>
+      <c r="BO26" s="5" t="n"/>
+      <c r="BP26" s="5" t="n"/>
+      <c r="BQ26" s="5" t="n"/>
+      <c r="BR26" s="5" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">

</xml_diff>

<commit_message>
data management script file restructure
</commit_message>
<xml_diff>
--- a/Docs/CorrectionStatus.xlsx
+++ b/Docs/CorrectionStatus.xlsx
@@ -50,8 +50,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00444444"/>
-        <bgColor rgb="00444444"/>
+        <fgColor rgb="00888888"/>
+        <bgColor rgb="00888888"/>
       </patternFill>
     </fill>
   </fills>

</xml_diff>